<commit_message>
add explanation of score and type
</commit_message>
<xml_diff>
--- a/CVE_Chrome.xlsx
+++ b/CVE_Chrome.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="13530" windowHeight="11715"/>
+    <workbookView windowWidth="27720" windowHeight="13320"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76">
   <si>
     <t>CVE</t>
   </si>
@@ -35,12 +35,19 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>CVE-2008-5749</t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>CVE-2008-5750</t>
@@ -57,6 +64,9 @@
   </si>
   <si>
     <t>script</t>
+  </si>
+  <si>
+    <t>score是根据poc内容的介绍详细程度进行打分1-5（1代表不可能重现  5代表最有可能重现 1-5代表重现可能性依次递增）；TYPE有script和core两种，script代表此缺陷是脚本缺陷，core代表此缺陷是浏览器内核缺陷</t>
   </si>
   <si>
     <t>CVE-2008-4340</t>
@@ -257,11 +267,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="24">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -285,20 +295,6 @@
     </font>
     <font>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -313,9 +309,24 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -329,21 +340,15 @@
     <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -357,6 +362,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -374,6 +394,36 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -381,38 +431,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -426,37 +445,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
+      <charset val="134"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -465,31 +460,157 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,67 +622,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -573,19 +640,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -595,62 +650,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -659,11 +660,100 @@
       <diagonal/>
     </border>
     <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -687,30 +777,6 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -756,160 +822,175 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="30" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -925,15 +1006,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
@@ -943,14 +1021,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="50">
@@ -1268,18 +1373,19 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="25.5555555555556" customWidth="1"/>
     <col min="3" max="3" width="12.4444444444444" style="2" customWidth="1"/>
     <col min="4" max="4" width="10.6666666666667"/>
     <col min="5" max="5" width="17.5555555555556" style="3" customWidth="1"/>
+    <col min="13" max="13" width="48.8888888888889" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="1" customFormat="1" ht="14.25" customHeight="1" spans="1:7">
@@ -1295,7 +1401,7 @@
       <c r="D1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
@@ -1305,584 +1411,605 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" ht="25.5" spans="1:7">
+    <row r="2" ht="25.5" spans="1:13">
       <c r="A2" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="8">
+      <c r="D2" s="7">
         <v>39805</v>
       </c>
-      <c r="E2" s="10" t="s">
+      <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="10">
         <v>3</v>
       </c>
-      <c r="G2" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" ht="25.5" spans="1:7">
+      <c r="G2" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="19"/>
+    </row>
+    <row r="3" ht="25.5" spans="1:13">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="8">
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="7">
         <v>39715</v>
       </c>
-      <c r="E3" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="11">
+      <c r="E3" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="10">
         <v>2</v>
       </c>
-      <c r="G3" s="12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" ht="25.5" spans="1:7">
+      <c r="G3" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="16"/>
+      <c r="K3" s="16"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="20"/>
+    </row>
+    <row r="4" ht="26.25" spans="1:13">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="8">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="7">
         <v>40838</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="F4" s="11">
+      <c r="E4" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="10">
         <v>2</v>
       </c>
-      <c r="G4" s="12" t="s">
-        <v>10</v>
-      </c>
+      <c r="G4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="17"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="21"/>
     </row>
     <row r="5" ht="25.5" spans="1:7">
       <c r="A5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="8">
+        <v>13</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" s="7">
         <v>39777</v>
       </c>
-      <c r="E5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="11">
+      <c r="E5" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" s="10">
         <v>3</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="6" ht="25.5" spans="1:7">
       <c r="A6" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B6" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="8">
+      <c r="C6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="7">
         <v>39742</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="11">
+      <c r="E6" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="10">
         <v>2</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="7" ht="25.5" spans="1:7">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="8">
+        <v>13</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="7">
         <v>39695</v>
       </c>
-      <c r="E7" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="11">
+      <c r="E7" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F7" s="10">
         <v>3</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" ht="25.5" spans="1:7">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B8" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" s="8">
+      <c r="C8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="7">
         <v>39696</v>
       </c>
-      <c r="E8" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="F8" s="11">
+      <c r="E8" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F8" s="10">
         <v>2</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="25.5" spans="1:7">
       <c r="A9" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D9" s="8">
+        <v>13</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="7">
         <v>39696</v>
       </c>
-      <c r="E9" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="11">
+      <c r="E9" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="10">
         <v>2</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="10" ht="25.5" spans="1:7">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10" s="8">
+      <c r="C10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="7">
         <v>39694</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="11">
+      <c r="E10" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="F10" s="10">
         <v>2</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" ht="25.5" spans="1:7">
       <c r="A11" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="8">
+        <v>13</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="7">
         <v>39694</v>
       </c>
-      <c r="E11" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="F11" s="11">
+      <c r="E11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="10">
         <v>3</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" ht="25.5" spans="1:7">
       <c r="A12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D12" s="8">
+        <v>13</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="7">
         <v>39696</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="F12" s="11">
+      <c r="E12" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="10">
         <v>1</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="25.5" spans="1:7">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="8">
+        <v>13</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D13" s="7">
         <v>39719</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F13" s="11">
+      <c r="E13" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="10">
         <v>4</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" ht="25.5" spans="1:7">
       <c r="A14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="8">
+      <c r="C14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="7">
         <v>39818</v>
       </c>
-      <c r="E14" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F14" s="11">
+      <c r="E14" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F14" s="10">
         <v>2</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="15" ht="25.5" spans="1:7">
       <c r="A15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B15" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="D15" s="8">
+      <c r="C15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D15" s="7">
         <v>39841</v>
       </c>
-      <c r="E15" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="11">
+      <c r="E15" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="10">
         <v>1</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="16" ht="25.5" spans="1:7">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="8">
+      <c r="C16" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="7">
         <v>39843</v>
       </c>
-      <c r="E16" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F16" s="11">
+      <c r="E16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="F16" s="10">
         <v>3</v>
       </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="17" ht="25.5" spans="1:7">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D17" s="8">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D17" s="7">
         <v>39933</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F17" s="11">
+      <c r="E17" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="F17" s="10">
         <v>2</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="G17" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="18" ht="25.5" spans="1:7">
       <c r="A18" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18" s="8">
+        <v>13</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="7">
         <v>40178</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="F18" s="11">
+      <c r="E18" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F18" s="10">
         <v>2</v>
       </c>
-      <c r="G18" s="12" t="s">
+      <c r="G18" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="19" ht="25.5" spans="1:7">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C19" s="7" t="s">
-        <v>54</v>
-      </c>
-      <c r="D19" s="8">
+        <v>13</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" s="7">
         <v>40243</v>
       </c>
-      <c r="E19" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F19" s="11">
+      <c r="E19" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F19" s="10">
         <v>3</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="20" ht="25.5" spans="1:7">
       <c r="A20" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="D20" s="8">
+        <v>13</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20" s="7">
         <v>40270</v>
       </c>
-      <c r="E20" s="13" t="s">
-        <v>57</v>
-      </c>
-      <c r="F20" s="11">
+      <c r="E20" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="F20" s="10">
         <v>4</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="G20" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="21" ht="25.5" spans="1:7">
       <c r="A21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D21" s="8">
+      <c r="C21" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D21" s="7">
         <v>40317</v>
       </c>
-      <c r="E21" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F21" s="11">
+      <c r="E21" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="10">
         <v>1</v>
       </c>
-      <c r="G21" s="12" t="s">
+      <c r="G21" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="22" ht="25.5" spans="1:7">
       <c r="A22" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="7" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="8">
+        <v>13</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D22" s="7">
         <v>40299</v>
       </c>
-      <c r="E22" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F22" s="11">
+      <c r="E22" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F22" s="10">
         <v>3</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="23" ht="25.5" spans="1:7">
       <c r="A23" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="8">
+        <v>13</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D23" s="7">
         <v>40561</v>
       </c>
-      <c r="E23" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="F23" s="11">
+      <c r="E23" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="F23" s="10">
         <v>2</v>
       </c>
-      <c r="G23" s="12" t="s">
+      <c r="G23" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" ht="25.5" spans="1:7">
       <c r="A24" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C24" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D24" s="8">
+        <v>13</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" s="7">
         <v>40820</v>
       </c>
-      <c r="E24" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F24" s="11">
+      <c r="E24" s="12" t="s">
+        <v>68</v>
+      </c>
+      <c r="F24" s="10">
         <v>4</v>
       </c>
-      <c r="G24" s="12" t="s">
+      <c r="G24" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="25" ht="25.5" spans="3:7">
-      <c r="C25" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="8">
+      <c r="C25" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="7">
         <v>42102</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="F25" s="11">
+      <c r="E25" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F25" s="10">
         <v>4</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="G25" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="26" ht="25.5" spans="3:7">
-      <c r="C26" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="D26" s="8">
+      <c r="C26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" s="7">
         <v>42188</v>
       </c>
-      <c r="E26" s="10" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" s="11">
+      <c r="E26" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="10">
         <v>4</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="G26" s="11" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="27" ht="25.5" spans="3:7">
-      <c r="C27" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="E27" s="13" t="s">
+      <c r="C27" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="F27" s="11">
+      <c r="E27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="10">
         <v>4</v>
       </c>
-      <c r="G27" s="12" t="s">
-        <v>74</v>
+      <c r="G27" s="11" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="I2:M4"/>
+  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="Remote" tooltip="https://www.exploit-db.com/remote/"/>
     <hyperlink ref="A3" r:id="rId2" display="CVE-2008-4340" tooltip="https://cve.mitre.org/cgi-bin/cvename.cgi?name=CVE-2008-4340"/>

</xml_diff>